<commit_message>
conducted unittest and testing plan 1, 2, 3, and 4. Update new data.
</commit_message>
<xml_diff>
--- a/examples/input/models/ModelB_discrete_biorecipe.xlsx
+++ b/examples/input/models/ModelB_discrete_biorecipe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasmine/Desktop/github_local_copy/VIOLIN/examples/input/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE24E97-FFBB-2040-9454-152BEAF97550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124921EF-2830-274A-B69E-8780F222EF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="3720" windowWidth="30980" windowHeight="19120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5880" yWindow="1480" windowWidth="30980" windowHeight="19120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="193">
   <si>
     <t>TCR</t>
   </si>
@@ -604,6 +604,9 @@
   </si>
   <si>
     <t>IL2_pn_nan_nan,IL2_pn_nan_go0005576</t>
+  </si>
+  <si>
+    <t>D,D,D,D</t>
   </si>
 </sst>
 </file>
@@ -1006,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P53" sqref="P53"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1575,7 +1578,7 @@
         <v>165</v>
       </c>
       <c r="O11" t="s">
-        <v>152</v>
+        <v>192</v>
       </c>
       <c r="Z11" t="s">
         <v>88</v>
@@ -1622,7 +1625,7 @@
         <v>190</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>152</v>
+        <v>192</v>
       </c>
       <c r="R12" s="2" t="s">
         <v>187</v>
@@ -3041,12 +3044,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A5F0FAD8EF73D449B39728944A2FE003" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eda1eed5f720a743d7e8e0702734e720">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1cab681b-ff41-4914-9116-6da4adaac831" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2c79a46b8f091c582d0b416678c62e2e" ns2:_="">
     <xsd:import namespace="1cab681b-ff41-4914-9116-6da4adaac831"/>
@@ -3184,6 +3181,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88E0DE6F-A777-40E1-A247-169523693BB9}">
   <ds:schemaRefs>
@@ -3193,15 +3196,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F179D896-5546-4B0D-A21A-6E2AE9122C3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03D04DA5-A0CE-49F7-B9AE-1669786C8B24}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3217,4 +3211,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F179D896-5546-4B0D-A21A-6E2AE9122C3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>